<commit_message>
added codepage handling added test for reading an object
wip
</commit_message>
<xml_diff>
--- a/test/configuration_test/producten1.xlsx
+++ b/test/configuration_test/producten1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ernstvorsteveld/git/dotnet/spreadsheet-reader/test/configuration_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55FDADCB-F238-4346-AB5C-D7447B7E0D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB144E9-D4E3-0648-A672-5B8C503B7EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="1600" windowWidth="27240" windowHeight="16440" xr2:uid="{3DA54F20-598F-4E4A-8E5D-79CB6B7B0683}"/>
   </bookViews>
@@ -543,11 +543,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879FBC09-EC5D-C84C-A804-4883ED0409CD}">
   <dimension ref="A1:AU17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="3.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>